<commit_message>
update 1128 y-time axis.
</commit_message>
<xml_diff>
--- a/baron_log.xlsx
+++ b/baron_log.xlsx
@@ -1,6 +1,6 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24527"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\seito\Documents\Baron-log\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{ED0DD637-A101-457A-9AAA-1B29297C1503}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{237411AA-23BC-49C3-8AB8-F1665F966D09}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="baron_log" sheetId="1" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="19" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -991,11 +991,12 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E122"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:E1048576"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A103" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A165" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18" x14ac:dyDescent="0.55000000000000004"/>
@@ -2350,6 +2351,641 @@
         <v>1</v>
       </c>
     </row>
+    <row r="123" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A123" s="1">
+        <v>44524</v>
+      </c>
+      <c r="B123" s="2">
+        <v>0.29166666666666669</v>
+      </c>
+      <c r="C123">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="124" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A124" s="1">
+        <v>44524</v>
+      </c>
+      <c r="B124" s="2">
+        <v>0.29236111111111113</v>
+      </c>
+      <c r="D124">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="125" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A125" s="1">
+        <v>44524</v>
+      </c>
+      <c r="B125" s="2">
+        <v>0.31597222222222221</v>
+      </c>
+      <c r="E125">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="126" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A126" s="1">
+        <v>44524</v>
+      </c>
+      <c r="B126" s="2">
+        <v>0.39583333333333331</v>
+      </c>
+    </row>
+    <row r="127" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A127" s="1">
+        <v>44524</v>
+      </c>
+      <c r="B127" s="2">
+        <v>0.47638888888888892</v>
+      </c>
+    </row>
+    <row r="128" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A128" s="1">
+        <v>44524</v>
+      </c>
+      <c r="B128" s="2">
+        <v>0.48541666666666666</v>
+      </c>
+      <c r="D128">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="129" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A129" s="1">
+        <v>44524</v>
+      </c>
+      <c r="B129" s="2">
+        <v>0.4861111111111111</v>
+      </c>
+      <c r="E129">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="130" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A130" s="1">
+        <v>44524</v>
+      </c>
+      <c r="B130" s="2">
+        <v>0.60763888888888895</v>
+      </c>
+      <c r="C130">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="131" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A131" s="1">
+        <v>44524</v>
+      </c>
+      <c r="B131" s="2">
+        <v>0.61319444444444449</v>
+      </c>
+      <c r="C131">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="132" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A132" s="1">
+        <v>44524</v>
+      </c>
+      <c r="B132" s="2">
+        <v>0.71527777777777779</v>
+      </c>
+      <c r="C132">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="133" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A133" s="1">
+        <v>44524</v>
+      </c>
+      <c r="B133" s="2">
+        <v>0.77083333333333337</v>
+      </c>
+      <c r="C133">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="134" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A134" s="1">
+        <v>44524</v>
+      </c>
+      <c r="B134" s="2">
+        <v>0.79166666666666663</v>
+      </c>
+      <c r="E134">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="135" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A135" s="1">
+        <v>44524</v>
+      </c>
+      <c r="B135" s="2">
+        <v>0.79513888888888884</v>
+      </c>
+      <c r="C135">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="136" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A136" s="1">
+        <v>44524</v>
+      </c>
+      <c r="B136" s="2">
+        <v>0.79861111111111116</v>
+      </c>
+      <c r="D136">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="137" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A137" s="1">
+        <v>44524</v>
+      </c>
+      <c r="B137" s="2">
+        <v>0.84791666666666676</v>
+      </c>
+      <c r="C137">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="138" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A138" s="1">
+        <v>44524</v>
+      </c>
+      <c r="B138" s="2">
+        <v>0.85138888888888886</v>
+      </c>
+      <c r="D138">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="139" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A139" s="1">
+        <v>44525</v>
+      </c>
+      <c r="B139" s="2">
+        <v>0.24305555555555555</v>
+      </c>
+      <c r="C139">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="140" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A140" s="1">
+        <v>44525</v>
+      </c>
+      <c r="B140" s="2">
+        <v>0.3</v>
+      </c>
+      <c r="E140">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="141" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A141" s="1">
+        <v>44525</v>
+      </c>
+      <c r="B141" s="2">
+        <v>0.31527777777777777</v>
+      </c>
+      <c r="D141">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="142" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A142" s="1">
+        <v>44525</v>
+      </c>
+      <c r="B142" s="2">
+        <v>0.45833333333333331</v>
+      </c>
+      <c r="C142">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="143" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A143" s="1">
+        <v>44525</v>
+      </c>
+      <c r="B143" s="2">
+        <v>0.47222222222222227</v>
+      </c>
+      <c r="E143">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="144" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A144" s="1">
+        <v>44525</v>
+      </c>
+      <c r="B144" s="2">
+        <v>0.4826388888888889</v>
+      </c>
+      <c r="C144">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="145" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A145" s="1">
+        <v>44525</v>
+      </c>
+      <c r="B145" s="2">
+        <v>0.48333333333333334</v>
+      </c>
+      <c r="D145">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="146" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A146" s="1">
+        <v>44525</v>
+      </c>
+      <c r="B146" s="2">
+        <v>0.60763888888888895</v>
+      </c>
+      <c r="C146">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="147" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A147" s="1">
+        <v>44525</v>
+      </c>
+      <c r="B147" s="2">
+        <v>0.76388888888888884</v>
+      </c>
+      <c r="C147">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="148" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A148" s="1">
+        <v>44525</v>
+      </c>
+      <c r="B148" s="2">
+        <v>0.79166666666666663</v>
+      </c>
+      <c r="E148">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="149" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A149" s="1">
+        <v>44525</v>
+      </c>
+      <c r="B149" s="2">
+        <v>0.8125</v>
+      </c>
+      <c r="D149">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="150" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A150" s="1">
+        <v>44525</v>
+      </c>
+      <c r="B150" s="2">
+        <v>0.90625</v>
+      </c>
+      <c r="C150">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="151" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A151" s="1">
+        <v>44526</v>
+      </c>
+      <c r="B151" s="2">
+        <v>0.17361111111111113</v>
+      </c>
+      <c r="C151">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="152" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A152" s="1">
+        <v>44526</v>
+      </c>
+      <c r="B152" s="2">
+        <v>0.30763888888888891</v>
+      </c>
+      <c r="C152">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="153" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A153" s="1">
+        <v>44526</v>
+      </c>
+      <c r="B153" s="2">
+        <v>0.3125</v>
+      </c>
+      <c r="E153">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="154" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A154" s="1">
+        <v>44526</v>
+      </c>
+      <c r="B154" s="2">
+        <v>0.34375</v>
+      </c>
+      <c r="C154">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="155" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A155" s="1">
+        <v>44526</v>
+      </c>
+      <c r="B155" s="2">
+        <v>0.34722222222222227</v>
+      </c>
+      <c r="D155">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="156" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A156" s="1">
+        <v>44526</v>
+      </c>
+      <c r="B156" s="2">
+        <v>0.41597222222222219</v>
+      </c>
+      <c r="C156">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="157" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A157" s="1">
+        <v>44526</v>
+      </c>
+      <c r="B157" s="2">
+        <v>0.50069444444444444</v>
+      </c>
+      <c r="C157">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="158" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A158" s="1">
+        <v>44526</v>
+      </c>
+      <c r="B158" s="2">
+        <v>0.53888888888888886</v>
+      </c>
+      <c r="E158">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="159" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A159" s="1">
+        <v>44526</v>
+      </c>
+      <c r="B159" s="2">
+        <v>0.54583333333333328</v>
+      </c>
+      <c r="C159">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="160" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A160" s="1">
+        <v>44526</v>
+      </c>
+      <c r="B160" s="2">
+        <v>0.5625</v>
+      </c>
+      <c r="D160">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="161" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A161" s="1">
+        <v>44526</v>
+      </c>
+      <c r="B161" s="2">
+        <v>0.61388888888888882</v>
+      </c>
+      <c r="C161">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="162" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A162" s="1">
+        <v>44526</v>
+      </c>
+      <c r="B162" s="2">
+        <v>0.67361111111111116</v>
+      </c>
+      <c r="C162">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="163" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A163" s="1">
+        <v>44526</v>
+      </c>
+      <c r="B163" s="2">
+        <v>0.74444444444444446</v>
+      </c>
+      <c r="C163">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="164" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A164" s="1">
+        <v>44526</v>
+      </c>
+      <c r="B164" s="2">
+        <v>0.79513888888888884</v>
+      </c>
+      <c r="E164">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="165" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A165" s="1">
+        <v>44526</v>
+      </c>
+      <c r="B165" s="2">
+        <v>0.80208333333333337</v>
+      </c>
+      <c r="C165">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="166" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A166" s="1">
+        <v>44526</v>
+      </c>
+      <c r="B166" s="2">
+        <v>0.81180555555555556</v>
+      </c>
+      <c r="D166">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="167" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A167" s="1">
+        <v>44526</v>
+      </c>
+      <c r="B167" s="2">
+        <v>0.86388888888888893</v>
+      </c>
+      <c r="C167">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="168" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A168" s="1">
+        <v>44526</v>
+      </c>
+      <c r="B168" s="2">
+        <v>0.89583333333333337</v>
+      </c>
+      <c r="C168">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="169" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A169" s="1">
+        <v>44527</v>
+      </c>
+      <c r="B169" s="2">
+        <v>0.26874999999999999</v>
+      </c>
+      <c r="C169">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="170" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A170" s="1">
+        <v>44527</v>
+      </c>
+      <c r="B170" s="2">
+        <v>0.27777777777777779</v>
+      </c>
+      <c r="E170">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="171" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A171" s="1">
+        <v>44527</v>
+      </c>
+      <c r="B171" s="2">
+        <v>0.28055555555555556</v>
+      </c>
+      <c r="C171">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="172" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A172" s="1">
+        <v>44527</v>
+      </c>
+      <c r="B172" s="2">
+        <v>0.42430555555555555</v>
+      </c>
+      <c r="C172">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="173" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A173" s="1">
+        <v>44527</v>
+      </c>
+      <c r="B173" s="2">
+        <v>0.45833333333333331</v>
+      </c>
+      <c r="C173">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="174" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A174" s="1">
+        <v>44527</v>
+      </c>
+      <c r="B174" s="2">
+        <v>0.56597222222222221</v>
+      </c>
+      <c r="C174">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="175" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A175" s="1">
+        <v>44527</v>
+      </c>
+      <c r="B175" s="2">
+        <v>0.60416666666666663</v>
+      </c>
+      <c r="C175">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="176" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A176" s="1">
+        <v>44527</v>
+      </c>
+      <c r="B176" s="2">
+        <v>0.65625</v>
+      </c>
+      <c r="C176">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="177" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A177" s="1">
+        <v>44527</v>
+      </c>
+      <c r="B177" s="2">
+        <v>0.73541666666666661</v>
+      </c>
+      <c r="C177">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="178" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A178" s="1">
+        <v>44527</v>
+      </c>
+      <c r="B178" s="2">
+        <v>0.75347222222222221</v>
+      </c>
+      <c r="D178">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="179" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A179" s="1">
+        <v>44527</v>
+      </c>
+      <c r="B179" s="2">
+        <v>0.77777777777777779</v>
+      </c>
+      <c r="E179">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="180" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A180" s="1">
+        <v>44527</v>
+      </c>
+      <c r="B180" s="2">
+        <v>0.78472222222222221</v>
+      </c>
+      <c r="C180">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="1048576" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A1048576" s="1"/>
+    </row>
   </sheetData>
   <phoneticPr fontId="18"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
start to develop the app.
</commit_message>
<xml_diff>
--- a/baron_log.xlsx
+++ b/baron_log.xlsx
@@ -8,19 +8,28 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\seito\Documents\Baron-log\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{237411AA-23BC-49C3-8AB8-F1665F966D09}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8A5E5221-B416-4D99-967A-82133BC3AAFB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="baron_log" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="11">
   <si>
     <t>date</t>
   </si>
@@ -35,6 +44,30 @@
   </si>
   <si>
     <t>Gohan</t>
+  </si>
+  <si>
+    <t>in-out</t>
+    <phoneticPr fontId="18"/>
+  </si>
+  <si>
+    <t>i</t>
+    <phoneticPr fontId="18"/>
+  </si>
+  <si>
+    <t>o</t>
+    <phoneticPr fontId="18"/>
+  </si>
+  <si>
+    <t>notes</t>
+    <phoneticPr fontId="18"/>
+  </si>
+  <si>
+    <t>new-toilet</t>
+    <phoneticPr fontId="18"/>
+  </si>
+  <si>
+    <t>old-toilet</t>
+    <phoneticPr fontId="18"/>
   </si>
 </sst>
 </file>
@@ -992,11 +1025,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E1048576"/>
+  <dimension ref="A1:G261"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A165" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18" x14ac:dyDescent="0.55000000000000004"/>
@@ -1006,7 +1039,7 @@
     <col min="3" max="5" width="14.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1022,8 +1055,14 @@
       <c r="E1" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="F1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" s="1">
         <v>44515</v>
       </c>
@@ -1034,7 +1073,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" s="1">
         <v>44515</v>
       </c>
@@ -1045,7 +1084,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" s="1">
         <v>44515</v>
       </c>
@@ -1056,7 +1095,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A5" s="1">
         <v>44515</v>
       </c>
@@ -1067,7 +1106,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A6" s="1">
         <v>44515</v>
       </c>
@@ -1078,7 +1117,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A7" s="1">
         <v>44515</v>
       </c>
@@ -1089,7 +1128,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A8" s="1">
         <v>44516</v>
       </c>
@@ -1100,7 +1139,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A9" s="1">
         <v>44516</v>
       </c>
@@ -1111,7 +1150,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A10" s="1">
         <v>44516</v>
       </c>
@@ -1122,7 +1161,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A11" s="1">
         <v>44516</v>
       </c>
@@ -1133,7 +1172,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A12" s="1">
         <v>44516</v>
       </c>
@@ -1144,7 +1183,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A13" s="1">
         <v>44516</v>
       </c>
@@ -1155,7 +1194,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A14" s="1">
         <v>44516</v>
       </c>
@@ -1166,7 +1205,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A15" s="1">
         <v>44516</v>
       </c>
@@ -1177,7 +1216,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A16" s="1">
         <v>44516</v>
       </c>
@@ -2939,7 +2978,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="177" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="177" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A177" s="1">
         <v>44527</v>
       </c>
@@ -2950,7 +2989,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="178" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="178" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A178" s="1">
         <v>44527</v>
       </c>
@@ -2961,7 +3000,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="179" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="179" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A179" s="1">
         <v>44527</v>
       </c>
@@ -2972,7 +3011,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="180" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="180" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A180" s="1">
         <v>44527</v>
       </c>
@@ -2983,8 +3022,923 @@
         <v>0</v>
       </c>
     </row>
-    <row r="1048576" spans="1:1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A1048576" s="1"/>
+    <row r="181" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A181" s="1">
+        <v>44528</v>
+      </c>
+      <c r="B181" s="2">
+        <v>0.27083333333333331</v>
+      </c>
+      <c r="C181">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="182" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A182" s="1">
+        <v>44528</v>
+      </c>
+      <c r="B182" s="2">
+        <v>0.3263888888888889</v>
+      </c>
+      <c r="C182">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="183" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A183" s="1">
+        <v>44528</v>
+      </c>
+      <c r="B183" s="2">
+        <v>0.34722222222222227</v>
+      </c>
+      <c r="E183">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="184" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A184" s="1">
+        <v>44528</v>
+      </c>
+      <c r="B184" s="2">
+        <v>0.35416666666666669</v>
+      </c>
+      <c r="D184">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="185" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A185" s="1">
+        <v>44528</v>
+      </c>
+      <c r="B185" s="2">
+        <v>0.36805555555555558</v>
+      </c>
+      <c r="C185">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="186" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A186" s="1">
+        <v>44528</v>
+      </c>
+      <c r="B186" s="2">
+        <v>0.39583333333333331</v>
+      </c>
+      <c r="C186">
+        <v>1</v>
+      </c>
+      <c r="F186" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="187" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A187" s="1">
+        <v>44528</v>
+      </c>
+      <c r="B187" s="2">
+        <v>0.41944444444444445</v>
+      </c>
+      <c r="C187">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="188" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A188" s="1">
+        <v>44528</v>
+      </c>
+      <c r="B188" s="2">
+        <v>0.4993055555555555</v>
+      </c>
+      <c r="C188">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="189" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A189" s="1">
+        <v>44528</v>
+      </c>
+      <c r="B189" s="2">
+        <v>0.61111111111111105</v>
+      </c>
+      <c r="D189">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="190" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A190" s="1">
+        <v>44528</v>
+      </c>
+      <c r="B190" s="2">
+        <v>0.79861111111111116</v>
+      </c>
+      <c r="E190">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="191" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A191" s="1">
+        <v>44528</v>
+      </c>
+      <c r="B191" s="2">
+        <v>0.80902777777777779</v>
+      </c>
+      <c r="C191">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="192" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A192" s="1">
+        <v>44529</v>
+      </c>
+      <c r="B192" s="2">
+        <v>0.11597222222222221</v>
+      </c>
+      <c r="C192">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="193" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A193" s="1">
+        <v>44529</v>
+      </c>
+      <c r="B193" s="2">
+        <v>0.3125</v>
+      </c>
+      <c r="D193">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="194" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A194" s="1">
+        <v>44529</v>
+      </c>
+      <c r="B194" s="2">
+        <v>0.31597222222222221</v>
+      </c>
+      <c r="C194">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="195" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A195" s="1">
+        <v>44529</v>
+      </c>
+      <c r="B195" s="2">
+        <v>0.31944444444444448</v>
+      </c>
+      <c r="E195">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="196" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A196" s="1">
+        <v>44529</v>
+      </c>
+      <c r="B196" s="2">
+        <v>0.47222222222222227</v>
+      </c>
+      <c r="C196">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="197" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A197" s="1">
+        <v>44529</v>
+      </c>
+      <c r="B197" s="2">
+        <v>0.54513888888888895</v>
+      </c>
+      <c r="E197">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="198" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A198" s="1">
+        <v>44529</v>
+      </c>
+      <c r="B198" s="2">
+        <v>0.67708333333333337</v>
+      </c>
+      <c r="C198">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="199" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A199" s="1">
+        <v>44529</v>
+      </c>
+      <c r="B199" s="2">
+        <v>0.7583333333333333</v>
+      </c>
+      <c r="C199">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="200" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A200" s="1">
+        <v>44529</v>
+      </c>
+      <c r="B200" s="2">
+        <v>0.78472222222222221</v>
+      </c>
+      <c r="E200">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="201" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A201" s="1">
+        <v>44529</v>
+      </c>
+      <c r="B201" s="2">
+        <v>0.79513888888888884</v>
+      </c>
+      <c r="C201">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="202" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A202" s="1">
+        <v>44529</v>
+      </c>
+      <c r="B202" s="2">
+        <v>0.79861111111111116</v>
+      </c>
+      <c r="D202">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="203" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A203" s="1">
+        <v>44529</v>
+      </c>
+      <c r="B203" s="2">
+        <v>0.84722222222222221</v>
+      </c>
+      <c r="C203">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="204" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A204" s="1">
+        <v>44530</v>
+      </c>
+      <c r="B204" s="2">
+        <v>0.28472222222222221</v>
+      </c>
+      <c r="C204">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="205" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A205" s="1">
+        <v>44530</v>
+      </c>
+      <c r="B205" s="2">
+        <v>0.2986111111111111</v>
+      </c>
+      <c r="D205">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="206" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A206" s="1">
+        <v>44530</v>
+      </c>
+      <c r="B206" s="2">
+        <v>0.34722222222222227</v>
+      </c>
+      <c r="E206">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="207" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A207" s="1">
+        <v>44530</v>
+      </c>
+      <c r="B207" s="2">
+        <v>0.41805555555555557</v>
+      </c>
+      <c r="C207">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="208" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A208" s="1">
+        <v>44530</v>
+      </c>
+      <c r="B208" s="2">
+        <v>0.46180555555555558</v>
+      </c>
+      <c r="C208">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="209" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A209" s="1">
+        <v>44530</v>
+      </c>
+      <c r="B209" s="2">
+        <v>0.51388888888888895</v>
+      </c>
+      <c r="E209">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="210" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A210" s="1">
+        <v>44530</v>
+      </c>
+      <c r="B210" s="2">
+        <v>0.51527777777777783</v>
+      </c>
+      <c r="C210">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="211" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A211" s="1">
+        <v>44530</v>
+      </c>
+      <c r="B211" s="2">
+        <v>0.67013888888888884</v>
+      </c>
+      <c r="C211">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="212" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A212" s="1">
+        <v>44530</v>
+      </c>
+      <c r="B212" s="2">
+        <v>0.79513888888888884</v>
+      </c>
+      <c r="E212">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="213" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A213" s="1">
+        <v>44530</v>
+      </c>
+      <c r="B213" s="2">
+        <v>0.80902777777777779</v>
+      </c>
+      <c r="D213">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="214" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A214" s="1">
+        <v>44530</v>
+      </c>
+      <c r="B214" s="2">
+        <v>0.90625</v>
+      </c>
+      <c r="C214">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="215" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A215" s="1">
+        <v>44530</v>
+      </c>
+      <c r="B215" s="2">
+        <v>0.95833333333333337</v>
+      </c>
+      <c r="D215">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="216" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A216" s="1">
+        <v>44530</v>
+      </c>
+      <c r="B216" s="2">
+        <v>0.97916666666666663</v>
+      </c>
+      <c r="C216">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="217" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A217" s="1">
+        <v>44531</v>
+      </c>
+      <c r="B217" s="2">
+        <v>0.32291666666666669</v>
+      </c>
+      <c r="C217">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="218" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A218" s="1">
+        <v>44531</v>
+      </c>
+      <c r="B218" s="2">
+        <v>0.33055555555555555</v>
+      </c>
+      <c r="E218">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="219" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A219" s="1">
+        <v>44531</v>
+      </c>
+      <c r="B219" s="2">
+        <v>0.44791666666666669</v>
+      </c>
+      <c r="C219">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="220" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A220" s="1">
+        <v>44531</v>
+      </c>
+      <c r="B220" s="2">
+        <v>0.51041666666666663</v>
+      </c>
+      <c r="C220">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="221" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A221" s="1">
+        <v>44531</v>
+      </c>
+      <c r="B221" s="2">
+        <v>0.51388888888888895</v>
+      </c>
+      <c r="E221">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="222" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A222" s="1">
+        <v>44531</v>
+      </c>
+      <c r="B222" s="2">
+        <v>0.66527777777777775</v>
+      </c>
+      <c r="C222">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="223" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A223" s="1">
+        <v>44531</v>
+      </c>
+      <c r="B223" s="2">
+        <v>0.68055555555555547</v>
+      </c>
+      <c r="D223">
+        <v>1</v>
+      </c>
+      <c r="F223" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="224" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A224" s="1">
+        <v>44531</v>
+      </c>
+      <c r="B224" s="2">
+        <v>0.72222222222222221</v>
+      </c>
+      <c r="C224">
+        <v>1</v>
+      </c>
+      <c r="F224" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="225" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="A225" s="1">
+        <v>44531</v>
+      </c>
+      <c r="B225" s="2">
+        <v>0.8125</v>
+      </c>
+      <c r="E225">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="226" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="A226" s="1">
+        <v>44531</v>
+      </c>
+      <c r="B226" s="2">
+        <v>0.91111111111111109</v>
+      </c>
+      <c r="C226">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="227" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="A227" s="1">
+        <v>44531</v>
+      </c>
+      <c r="B227" s="2">
+        <v>0.91805555555555562</v>
+      </c>
+      <c r="D227">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="228" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="A228" s="1">
+        <v>44532</v>
+      </c>
+      <c r="B228" s="2">
+        <v>1.7361111111111112E-2</v>
+      </c>
+      <c r="C228">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="229" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="A229" s="1">
+        <v>44532</v>
+      </c>
+      <c r="B229" s="2">
+        <v>0.27083333333333331</v>
+      </c>
+      <c r="C229">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="230" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="A230" s="1">
+        <v>44532</v>
+      </c>
+      <c r="B230" s="2">
+        <v>0.27777777777777779</v>
+      </c>
+      <c r="D230">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="231" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="A231" s="1">
+        <v>44532</v>
+      </c>
+      <c r="B231" s="2">
+        <v>0.30555555555555552</v>
+      </c>
+      <c r="D231">
+        <v>1</v>
+      </c>
+      <c r="F231" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="232" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="A232" s="1">
+        <v>44532</v>
+      </c>
+      <c r="B232" s="2">
+        <v>0.3298611111111111</v>
+      </c>
+      <c r="E232">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="233" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="A233" s="1">
+        <v>44532</v>
+      </c>
+      <c r="B233" s="2">
+        <v>0.38541666666666669</v>
+      </c>
+      <c r="C233">
+        <v>0</v>
+      </c>
+      <c r="G233" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="234" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="A234" s="1">
+        <v>44532</v>
+      </c>
+      <c r="B234" s="2">
+        <v>0.44791666666666669</v>
+      </c>
+      <c r="C234">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="235" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="A235" s="1">
+        <v>44532</v>
+      </c>
+      <c r="B235" s="2">
+        <v>0.54027777777777775</v>
+      </c>
+      <c r="E235">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="236" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="A236" s="1">
+        <v>44532</v>
+      </c>
+      <c r="B236" s="2">
+        <v>0.8125</v>
+      </c>
+      <c r="C236">
+        <v>0</v>
+      </c>
+      <c r="G236" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="237" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="A237" s="1">
+        <v>44532</v>
+      </c>
+      <c r="B237" s="2">
+        <v>0.79513888888888884</v>
+      </c>
+      <c r="E237">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="238" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="A238" s="1">
+        <v>44532</v>
+      </c>
+      <c r="B238" s="2">
+        <v>0.80208333333333337</v>
+      </c>
+      <c r="C238">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="239" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="A239" s="1">
+        <v>44532</v>
+      </c>
+      <c r="B239" s="2">
+        <v>0.80902777777777779</v>
+      </c>
+      <c r="D239">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="240" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="A240" s="1">
+        <v>44532</v>
+      </c>
+      <c r="B240" s="2">
+        <v>0.90972222222222221</v>
+      </c>
+      <c r="C240">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="241" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A241" s="1">
+        <v>44533</v>
+      </c>
+      <c r="B241" s="2">
+        <v>0.20138888888888887</v>
+      </c>
+      <c r="C241">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="242" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A242" s="1">
+        <v>44533</v>
+      </c>
+      <c r="B242" s="2">
+        <v>0.30208333333333331</v>
+      </c>
+      <c r="C242">
+        <v>1</v>
+      </c>
+      <c r="F242" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="243" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A243" s="1">
+        <v>44533</v>
+      </c>
+      <c r="B243" s="2">
+        <v>0.31111111111111112</v>
+      </c>
+      <c r="D243">
+        <v>1</v>
+      </c>
+      <c r="F243" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="244" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A244" s="1">
+        <v>44533</v>
+      </c>
+      <c r="B244" s="2">
+        <v>0.42986111111111108</v>
+      </c>
+      <c r="C244">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="245" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A245" s="1">
+        <v>44533</v>
+      </c>
+      <c r="B245" s="2">
+        <v>0.53333333333333333</v>
+      </c>
+      <c r="E245">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="246" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A246" s="1">
+        <v>44533</v>
+      </c>
+      <c r="B246" s="2">
+        <v>0.5395833333333333</v>
+      </c>
+      <c r="C246">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="247" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A247" s="1">
+        <v>44533</v>
+      </c>
+      <c r="B247" s="2">
+        <v>0.54513888888888895</v>
+      </c>
+      <c r="D247">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="248" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A248" s="1">
+        <v>44533</v>
+      </c>
+      <c r="B248" s="2">
+        <v>0.76041666666666663</v>
+      </c>
+      <c r="C248">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="249" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A249" s="1">
+        <v>44533</v>
+      </c>
+      <c r="B249" s="2">
+        <v>0.77083333333333337</v>
+      </c>
+      <c r="C249">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="250" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A250" s="1">
+        <v>44533</v>
+      </c>
+      <c r="B250" s="2">
+        <v>0.84375</v>
+      </c>
+      <c r="D250">
+        <v>1</v>
+      </c>
+      <c r="F250" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="251" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A251" s="1">
+        <v>44533</v>
+      </c>
+      <c r="B251" s="2">
+        <v>0.86111111111111116</v>
+      </c>
+      <c r="E251">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="252" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A252" s="1">
+        <v>44533</v>
+      </c>
+      <c r="B252" s="2">
+        <v>0.93125000000000002</v>
+      </c>
+      <c r="C252">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="253" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A253" s="1">
+        <v>44534</v>
+      </c>
+      <c r="B253" s="2">
+        <v>0.20694444444444446</v>
+      </c>
+      <c r="C253">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="254" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A254" s="1">
+        <v>44534</v>
+      </c>
+      <c r="B254" s="2">
+        <v>0.30902777777777779</v>
+      </c>
+      <c r="E254">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="255" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A255" s="1">
+        <v>44534</v>
+      </c>
+      <c r="B255" s="2">
+        <v>0.35486111111111113</v>
+      </c>
+      <c r="D255">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="256" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A256" s="1">
+        <v>44534</v>
+      </c>
+      <c r="B256" s="2">
+        <v>0.44791666666666669</v>
+      </c>
+      <c r="C256">
+        <v>1</v>
+      </c>
+      <c r="F256" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="257" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A257" s="1">
+        <v>44534</v>
+      </c>
+      <c r="B257" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="D257">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="258" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A258" s="1">
+        <v>44534</v>
+      </c>
+      <c r="B258" s="2">
+        <v>0.52083333333333337</v>
+      </c>
+      <c r="E258">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="259" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A259" s="1">
+        <v>44534</v>
+      </c>
+      <c r="B259" s="2">
+        <v>0.65555555555555556</v>
+      </c>
+    </row>
+    <row r="260" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A260" s="1">
+        <v>44534</v>
+      </c>
+      <c r="B260" s="2">
+        <v>0.8222222222222223</v>
+      </c>
+      <c r="E260">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="261" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A261" s="1">
+        <v>44534</v>
+      </c>
+      <c r="B261" s="2">
+        <v>0.89583333333333337</v>
+      </c>
+      <c r="C261">
+        <v>0</v>
+      </c>
     </row>
   </sheetData>
   <phoneticPr fontId="18"/>

</xml_diff>

<commit_message>
update app show the success rate
</commit_message>
<xml_diff>
--- a/baron_log.xlsx
+++ b/baron_log.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24827"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\seito\Documents\Baron-log\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8A5E5221-B416-4D99-967A-82133BC3AAFB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{01517528-37B5-4FB0-A772-D6CB610A0C9E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -46,10 +46,6 @@
     <t>Gohan</t>
   </si>
   <si>
-    <t>in-out</t>
-    <phoneticPr fontId="18"/>
-  </si>
-  <si>
     <t>i</t>
     <phoneticPr fontId="18"/>
   </si>
@@ -67,6 +63,10 @@
   </si>
   <si>
     <t>old-toilet</t>
+    <phoneticPr fontId="18"/>
+  </si>
+  <si>
+    <t>out</t>
     <phoneticPr fontId="18"/>
   </si>
 </sst>
@@ -660,7 +660,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -668,6 +668,9 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="21" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -1025,11 +1028,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G261"/>
+  <dimension ref="A1:G380"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+      <pane ySplit="1" topLeftCell="A365" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18" x14ac:dyDescent="0.55000000000000004"/>
@@ -1056,10 +1059,10 @@
         <v>4</v>
       </c>
       <c r="F1" t="s">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="G1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.55000000000000004">
@@ -3088,7 +3091,7 @@
         <v>1</v>
       </c>
       <c r="F186" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="187" spans="1:6" x14ac:dyDescent="0.55000000000000004">
@@ -3498,7 +3501,7 @@
         <v>1</v>
       </c>
       <c r="F223" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="224" spans="1:6" x14ac:dyDescent="0.55000000000000004">
@@ -3512,7 +3515,7 @@
         <v>1</v>
       </c>
       <c r="F224" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="225" spans="1:7" x14ac:dyDescent="0.55000000000000004">
@@ -3592,7 +3595,7 @@
         <v>1</v>
       </c>
       <c r="F231" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="232" spans="1:7" x14ac:dyDescent="0.55000000000000004">
@@ -3617,7 +3620,7 @@
         <v>0</v>
       </c>
       <c r="G233" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="234" spans="1:7" x14ac:dyDescent="0.55000000000000004">
@@ -3653,7 +3656,7 @@
         <v>0</v>
       </c>
       <c r="G236" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="237" spans="1:7" x14ac:dyDescent="0.55000000000000004">
@@ -3722,7 +3725,7 @@
         <v>1</v>
       </c>
       <c r="F242" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="243" spans="1:6" x14ac:dyDescent="0.55000000000000004">
@@ -3736,7 +3739,7 @@
         <v>1</v>
       </c>
       <c r="F243" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="244" spans="1:6" x14ac:dyDescent="0.55000000000000004">
@@ -3816,7 +3819,7 @@
         <v>1</v>
       </c>
       <c r="F250" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="251" spans="1:6" x14ac:dyDescent="0.55000000000000004">
@@ -3885,10 +3888,10 @@
         <v>1</v>
       </c>
       <c r="F256" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="257" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="257" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A257" s="1">
         <v>44534</v>
       </c>
@@ -3899,7 +3902,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="258" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="258" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A258" s="1">
         <v>44534</v>
       </c>
@@ -3910,7 +3913,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="259" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="259" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A259" s="1">
         <v>44534</v>
       </c>
@@ -3918,7 +3921,7 @@
         <v>0.65555555555555556</v>
       </c>
     </row>
-    <row r="260" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="260" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A260" s="1">
         <v>44534</v>
       </c>
@@ -3929,7 +3932,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="261" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="261" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A261" s="1">
         <v>44534</v>
       </c>
@@ -3938,6 +3941,1372 @@
       </c>
       <c r="C261">
         <v>0</v>
+      </c>
+    </row>
+    <row r="262" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A262" s="1">
+        <v>44590</v>
+      </c>
+      <c r="B262" s="2">
+        <v>0.36805555555555558</v>
+      </c>
+      <c r="C262">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="263" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A263" s="1">
+        <v>44590</v>
+      </c>
+      <c r="B263" s="2">
+        <v>0.375</v>
+      </c>
+      <c r="D263">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="264" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A264" s="1">
+        <v>44590</v>
+      </c>
+      <c r="B264" s="2">
+        <v>0.41666666666666669</v>
+      </c>
+      <c r="D264">
+        <v>1</v>
+      </c>
+      <c r="F264">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="265" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A265" s="1">
+        <v>44590</v>
+      </c>
+      <c r="B265" s="2">
+        <v>0.42708333333333331</v>
+      </c>
+      <c r="C265">
+        <v>1</v>
+      </c>
+      <c r="F265">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="266" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A266" s="1">
+        <v>44590</v>
+      </c>
+      <c r="B266" s="2">
+        <v>0.49305555555555558</v>
+      </c>
+      <c r="E266">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="267" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A267" s="1">
+        <v>44590</v>
+      </c>
+      <c r="B267" s="2">
+        <v>0.57638888888888895</v>
+      </c>
+      <c r="C267">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="268" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A268" s="1">
+        <v>44590</v>
+      </c>
+      <c r="B268" s="2">
+        <v>0.77777777777777779</v>
+      </c>
+      <c r="E268">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="269" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A269" s="1">
+        <v>44590</v>
+      </c>
+      <c r="B269" s="2">
+        <v>0.83333333333333337</v>
+      </c>
+      <c r="C269">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="270" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A270" s="1">
+        <v>44590</v>
+      </c>
+      <c r="B270" s="2">
+        <v>0.99861111111111101</v>
+      </c>
+      <c r="C270">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="271" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A271" s="1">
+        <v>44591</v>
+      </c>
+      <c r="B271" s="2">
+        <v>0.37847222222222227</v>
+      </c>
+      <c r="C271">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="272" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A272" s="1">
+        <v>44591</v>
+      </c>
+      <c r="B272" s="2">
+        <v>0.3888888888888889</v>
+      </c>
+      <c r="D272">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="273" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A273" s="1">
+        <v>44591</v>
+      </c>
+      <c r="B273" s="2">
+        <v>0.40138888888888885</v>
+      </c>
+      <c r="E273">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="274" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A274" s="1">
+        <v>44591</v>
+      </c>
+      <c r="B274" s="2">
+        <v>0.48958333333333331</v>
+      </c>
+      <c r="C274">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="275" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A275" s="1">
+        <v>44591</v>
+      </c>
+      <c r="B275" s="2">
+        <v>0.53472222222222221</v>
+      </c>
+      <c r="C275">
+        <v>1</v>
+      </c>
+      <c r="F275">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="276" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A276" s="1">
+        <v>44591</v>
+      </c>
+      <c r="B276" s="2">
+        <v>0.54166666666666663</v>
+      </c>
+      <c r="E276">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="277" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A277" s="1">
+        <v>44591</v>
+      </c>
+      <c r="B277" s="2">
+        <v>0.55208333333333337</v>
+      </c>
+      <c r="D277">
+        <v>1</v>
+      </c>
+      <c r="F277">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="278" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A278" s="1">
+        <v>44591</v>
+      </c>
+      <c r="B278" s="2">
+        <v>0.68472222222222223</v>
+      </c>
+      <c r="C278">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="279" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A279" s="1">
+        <v>44591</v>
+      </c>
+      <c r="B279" s="2">
+        <v>0.72916666666666663</v>
+      </c>
+      <c r="C279">
+        <v>1</v>
+      </c>
+      <c r="F279">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="280" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A280" s="1">
+        <v>44591</v>
+      </c>
+      <c r="B280" s="2">
+        <v>0.7583333333333333</v>
+      </c>
+      <c r="E280">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="281" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A281" s="1">
+        <v>44591</v>
+      </c>
+      <c r="B281" s="2">
+        <v>0.83333333333333337</v>
+      </c>
+      <c r="C281">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="282" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A282" s="1">
+        <v>44591</v>
+      </c>
+      <c r="B282" s="2">
+        <v>0.89583333333333337</v>
+      </c>
+      <c r="C282">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="283" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A283" s="1">
+        <v>44591</v>
+      </c>
+      <c r="B283" s="2">
+        <v>0.91666666666666663</v>
+      </c>
+      <c r="C283">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="284" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A284" s="1">
+        <v>44592</v>
+      </c>
+      <c r="B284" s="2">
+        <v>0.3125</v>
+      </c>
+      <c r="C284">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="285" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A285" s="1">
+        <v>44592</v>
+      </c>
+      <c r="B285" s="2">
+        <v>0.34027777777777773</v>
+      </c>
+      <c r="C285">
+        <v>1</v>
+      </c>
+      <c r="F285">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="286" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A286" s="1">
+        <v>44592</v>
+      </c>
+      <c r="B286" s="2">
+        <v>0.34722222222222227</v>
+      </c>
+      <c r="D286">
+        <v>1</v>
+      </c>
+      <c r="F286">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="287" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A287" s="1">
+        <v>44592</v>
+      </c>
+      <c r="B287" s="2">
+        <v>0.3611111111111111</v>
+      </c>
+      <c r="E287">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="288" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A288" s="1">
+        <v>44592</v>
+      </c>
+      <c r="B288" s="2">
+        <v>0.65972222222222221</v>
+      </c>
+      <c r="C288">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="289" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A289" s="1">
+        <v>44592</v>
+      </c>
+      <c r="B289" s="2">
+        <v>0.7895833333333333</v>
+      </c>
+      <c r="C289">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="290" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A290" s="1">
+        <v>44592</v>
+      </c>
+      <c r="B290" s="2">
+        <v>0.81944444444444453</v>
+      </c>
+      <c r="D290">
+        <v>1</v>
+      </c>
+      <c r="F290">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="291" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A291" s="1">
+        <v>44592</v>
+      </c>
+      <c r="B291" s="2">
+        <v>0.84027777777777779</v>
+      </c>
+      <c r="E291">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="292" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A292" s="1">
+        <v>44593</v>
+      </c>
+      <c r="B292" s="2">
+        <v>0.33680555555555558</v>
+      </c>
+      <c r="C292">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="293" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A293" s="1">
+        <v>44593</v>
+      </c>
+      <c r="B293" s="2">
+        <v>0.35416666666666669</v>
+      </c>
+      <c r="E293">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="294" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A294" s="1">
+        <v>44593</v>
+      </c>
+      <c r="B294" s="2">
+        <v>0.40972222222222227</v>
+      </c>
+      <c r="C294">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="295" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A295" s="1">
+        <v>44593</v>
+      </c>
+      <c r="B295" s="2">
+        <v>0.41319444444444442</v>
+      </c>
+      <c r="E295">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="296" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A296" s="1">
+        <v>44593</v>
+      </c>
+      <c r="B296" s="2">
+        <v>0.54861111111111105</v>
+      </c>
+      <c r="C296">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="297" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A297" s="1">
+        <v>44593</v>
+      </c>
+      <c r="B297" s="2">
+        <v>0.56597222222222221</v>
+      </c>
+      <c r="E297">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="298" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A298" s="1">
+        <v>44593</v>
+      </c>
+      <c r="B298" s="2">
+        <v>0.71458333333333324</v>
+      </c>
+      <c r="C298">
+        <v>1</v>
+      </c>
+      <c r="F298">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="299" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A299" s="1">
+        <v>44593</v>
+      </c>
+      <c r="B299" s="2">
+        <v>0.84027777777777779</v>
+      </c>
+      <c r="E299">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="300" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A300" s="1">
+        <v>44594</v>
+      </c>
+      <c r="B300" s="2">
+        <v>0.36805555555555558</v>
+      </c>
+      <c r="C300">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="301" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A301" s="1">
+        <v>44594</v>
+      </c>
+      <c r="B301" s="2">
+        <v>0.38194444444444442</v>
+      </c>
+      <c r="E301">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="302" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A302" s="1">
+        <v>44594</v>
+      </c>
+      <c r="B302" s="2">
+        <v>0.44305555555555554</v>
+      </c>
+      <c r="D302">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="303" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A303" s="1">
+        <v>44594</v>
+      </c>
+      <c r="B303" s="2">
+        <v>0.5083333333333333</v>
+      </c>
+      <c r="C303">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="304" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A304" s="1">
+        <v>44594</v>
+      </c>
+      <c r="B304" s="2">
+        <v>0.7993055555555556</v>
+      </c>
+      <c r="E304">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="305" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A305" s="1">
+        <v>44594</v>
+      </c>
+      <c r="B305" s="2">
+        <v>0.88541666666666663</v>
+      </c>
+      <c r="C305">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="306" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A306" s="1">
+        <v>44603</v>
+      </c>
+      <c r="B306" s="2">
+        <v>0.33680555555555558</v>
+      </c>
+      <c r="C306">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="307" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A307" s="1">
+        <v>44603</v>
+      </c>
+      <c r="B307" s="2">
+        <v>0.375</v>
+      </c>
+      <c r="E307">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="308" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A308" s="1">
+        <v>44603</v>
+      </c>
+      <c r="B308" s="2">
+        <v>0.42569444444444443</v>
+      </c>
+      <c r="D308">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="309" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A309" s="1">
+        <v>44603</v>
+      </c>
+      <c r="B309" s="2">
+        <v>0.52777777777777779</v>
+      </c>
+      <c r="D309">
+        <v>1</v>
+      </c>
+      <c r="F309">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="310" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A310" s="1">
+        <v>44603</v>
+      </c>
+      <c r="B310" s="2">
+        <v>0.54166666666666663</v>
+      </c>
+      <c r="E310">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="311" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A311" s="1">
+        <v>44603</v>
+      </c>
+      <c r="B311" s="2">
+        <v>0.63611111111111118</v>
+      </c>
+      <c r="C311">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="312" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A312" s="1">
+        <v>44603</v>
+      </c>
+      <c r="B312" s="2">
+        <v>0.79513888888888884</v>
+      </c>
+      <c r="C312">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="313" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A313" s="1">
+        <v>44604</v>
+      </c>
+      <c r="B313" s="2">
+        <v>0.375</v>
+      </c>
+      <c r="C313">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="314" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A314" s="1">
+        <v>44604</v>
+      </c>
+      <c r="B314" s="2">
+        <v>0.39583333333333331</v>
+      </c>
+      <c r="D314">
+        <v>1</v>
+      </c>
+      <c r="F314">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="315" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A315" s="1">
+        <v>44604</v>
+      </c>
+      <c r="B315" s="2">
+        <v>0.40486111111111112</v>
+      </c>
+      <c r="E315">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="316" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A316" s="1">
+        <v>44604</v>
+      </c>
+      <c r="B316" s="2">
+        <v>0.50347222222222221</v>
+      </c>
+      <c r="C316">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="317" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A317" s="1">
+        <v>44604</v>
+      </c>
+      <c r="B317" s="2">
+        <v>0.52777777777777779</v>
+      </c>
+      <c r="C317">
+        <v>1</v>
+      </c>
+      <c r="F317">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="318" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A318" s="1">
+        <v>44604</v>
+      </c>
+      <c r="B318" s="2">
+        <v>0.53125</v>
+      </c>
+      <c r="D318">
+        <v>1</v>
+      </c>
+      <c r="F318">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="319" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A319" s="1">
+        <v>44604</v>
+      </c>
+      <c r="B319" s="2">
+        <v>0.54861111111111105</v>
+      </c>
+      <c r="E319">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="320" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A320" s="1">
+        <v>44604</v>
+      </c>
+      <c r="B320" s="2">
+        <v>0.65972222222222221</v>
+      </c>
+      <c r="C320">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="321" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A321" s="1">
+        <v>44604</v>
+      </c>
+      <c r="B321" s="2">
+        <v>0.78125</v>
+      </c>
+      <c r="C321">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="322" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A322" s="1">
+        <v>44604</v>
+      </c>
+      <c r="B322" s="2">
+        <v>0.80069444444444438</v>
+      </c>
+      <c r="E322">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="323" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A323" s="1">
+        <v>44604</v>
+      </c>
+      <c r="B323" s="2">
+        <v>0.90833333333333333</v>
+      </c>
+      <c r="C323">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="324" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A324" s="1">
+        <v>44605</v>
+      </c>
+      <c r="B324" s="2">
+        <v>0.26041666666666669</v>
+      </c>
+      <c r="C324">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="325" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A325" s="1">
+        <v>44605</v>
+      </c>
+      <c r="B325" s="2">
+        <v>0.3298611111111111</v>
+      </c>
+      <c r="C325">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="326" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A326" s="1">
+        <v>44605</v>
+      </c>
+      <c r="B326" s="2">
+        <v>0.3576388888888889</v>
+      </c>
+      <c r="E326">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="327" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A327" s="1">
+        <v>44605</v>
+      </c>
+      <c r="B327" s="2">
+        <v>0.3923611111111111</v>
+      </c>
+      <c r="C327">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="328" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A328" s="1">
+        <v>44605</v>
+      </c>
+      <c r="B328" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="E328">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="329" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A329" s="1">
+        <v>44605</v>
+      </c>
+      <c r="B329" s="2">
+        <v>0.57361111111111118</v>
+      </c>
+      <c r="C329">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="330" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A330" s="1">
+        <v>44605</v>
+      </c>
+      <c r="B330" s="2">
+        <v>0.68819444444444444</v>
+      </c>
+      <c r="C330">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="331" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A331" s="1">
+        <v>44605</v>
+      </c>
+      <c r="B331" s="2">
+        <v>0.78541666666666676</v>
+      </c>
+      <c r="D331">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="332" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A332" s="1">
+        <v>44605</v>
+      </c>
+      <c r="B332" s="2">
+        <v>0.79166666666666663</v>
+      </c>
+      <c r="E332">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="333" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A333" s="1">
+        <v>44605</v>
+      </c>
+      <c r="B333" s="2">
+        <v>0.90625</v>
+      </c>
+      <c r="C333">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="334" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A334" s="1">
+        <v>44605</v>
+      </c>
+      <c r="B334" s="2">
+        <v>0.92499999999999993</v>
+      </c>
+      <c r="D334">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="335" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A335" s="1">
+        <v>44606</v>
+      </c>
+      <c r="B335" s="2">
+        <v>0.34722222222222227</v>
+      </c>
+      <c r="C335">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="336" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A336" s="1">
+        <v>44606</v>
+      </c>
+      <c r="B336" s="2">
+        <v>0.3527777777777778</v>
+      </c>
+      <c r="E336">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="337" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A337" s="1">
+        <v>44606</v>
+      </c>
+      <c r="B337" s="2">
+        <v>0.54166666666666663</v>
+      </c>
+      <c r="E337">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="338" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A338" s="1">
+        <v>44606</v>
+      </c>
+      <c r="B338" s="2">
+        <v>0.56944444444444442</v>
+      </c>
+      <c r="C338">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="339" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A339" s="1">
+        <v>44606</v>
+      </c>
+      <c r="B339" s="2">
+        <v>0.64652777777777781</v>
+      </c>
+      <c r="C339">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="340" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A340" s="1">
+        <v>44606</v>
+      </c>
+      <c r="B340" s="2">
+        <v>0.65069444444444446</v>
+      </c>
+      <c r="D340">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="341" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A341" s="1">
+        <v>44606</v>
+      </c>
+      <c r="B341" s="2">
+        <v>0.76388888888888884</v>
+      </c>
+      <c r="C341">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="342" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A342" s="1">
+        <v>44606</v>
+      </c>
+      <c r="B342" s="2">
+        <v>0.81597222222222221</v>
+      </c>
+      <c r="E342">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="343" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A343" s="1">
+        <v>44606</v>
+      </c>
+      <c r="B343" s="2">
+        <v>0.87013888888888891</v>
+      </c>
+      <c r="C343">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="344" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A344" s="1">
+        <v>44606</v>
+      </c>
+      <c r="B344" s="2">
+        <v>0.9145833333333333</v>
+      </c>
+      <c r="D344">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="345" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A345" s="1">
+        <v>44606</v>
+      </c>
+      <c r="B345" s="2">
+        <v>0.96180555555555547</v>
+      </c>
+      <c r="C345">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="346" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A346" s="1">
+        <v>44607</v>
+      </c>
+      <c r="B346" s="2">
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="C346">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="347" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A347" s="1">
+        <v>44607</v>
+      </c>
+      <c r="B347" s="2">
+        <v>0.34930555555555554</v>
+      </c>
+      <c r="E347">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="348" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A348" s="1">
+        <v>44607</v>
+      </c>
+      <c r="B348" s="2">
+        <v>0.38194444444444442</v>
+      </c>
+      <c r="C348">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="349" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A349" s="1">
+        <v>44607</v>
+      </c>
+      <c r="B349" s="2">
+        <v>0.40625</v>
+      </c>
+      <c r="D349">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="350" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A350" s="1">
+        <v>44607</v>
+      </c>
+      <c r="B350" s="2">
+        <v>0.49305555555555558</v>
+      </c>
+      <c r="E350">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="351" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A351" s="1">
+        <v>44608</v>
+      </c>
+      <c r="B351" s="2">
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="C351">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="352" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A352" s="1">
+        <v>44608</v>
+      </c>
+      <c r="B352" s="2">
+        <v>0.41666666666666669</v>
+      </c>
+      <c r="E352">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="353" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A353" s="1">
+        <v>44608</v>
+      </c>
+      <c r="B353" s="2">
+        <v>0.76874999999999993</v>
+      </c>
+      <c r="C353">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="354" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A354" s="1">
+        <v>44608</v>
+      </c>
+      <c r="B354" s="2">
+        <v>0.79166666666666663</v>
+      </c>
+      <c r="E354">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="355" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A355" s="1">
+        <v>44608</v>
+      </c>
+      <c r="B355" s="2">
+        <v>0.9472222222222223</v>
+      </c>
+      <c r="C355">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="356" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A356" s="1">
+        <v>44609</v>
+      </c>
+      <c r="B356" s="2">
+        <v>0.36527777777777781</v>
+      </c>
+      <c r="C356">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="357" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A357" s="1">
+        <v>44609</v>
+      </c>
+      <c r="B357" s="3">
+        <v>0.37152777777777773</v>
+      </c>
+      <c r="E357">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="358" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A358" s="1">
+        <v>44609</v>
+      </c>
+      <c r="B358" s="2">
+        <v>0.53819444444444442</v>
+      </c>
+      <c r="C358">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="359" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A359" s="1">
+        <v>44609</v>
+      </c>
+      <c r="B359" s="2">
+        <v>0.54513888888888895</v>
+      </c>
+      <c r="D359">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="360" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A360" s="1">
+        <v>44609</v>
+      </c>
+      <c r="B360" s="2">
+        <v>0.58680555555555558</v>
+      </c>
+      <c r="C360">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="361" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A361" s="1">
+        <v>44609</v>
+      </c>
+      <c r="B361" s="2">
+        <v>0.81319444444444444</v>
+      </c>
+      <c r="E361">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="362" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A362" s="1">
+        <v>44609</v>
+      </c>
+      <c r="B362" s="2">
+        <v>0.85069444444444453</v>
+      </c>
+      <c r="D362">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="363" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A363" s="1">
+        <v>44609</v>
+      </c>
+      <c r="B363" s="2">
+        <v>0.90972222222222221</v>
+      </c>
+      <c r="C363">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="364" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A364" s="1">
+        <v>44609</v>
+      </c>
+      <c r="B364" s="2">
+        <v>0.92361111111111116</v>
+      </c>
+      <c r="D364">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="365" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A365" s="1">
+        <v>44617</v>
+      </c>
+      <c r="B365" s="2">
+        <v>0.36458333333333331</v>
+      </c>
+      <c r="C365">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="366" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A366" s="1">
+        <v>44617</v>
+      </c>
+      <c r="B366" s="2">
+        <v>0.38194444444444442</v>
+      </c>
+      <c r="E366">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="367" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A367" s="1">
+        <v>44617</v>
+      </c>
+      <c r="B367" s="2">
+        <v>0.4861111111111111</v>
+      </c>
+      <c r="C367">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="368" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A368" s="1">
+        <v>44617</v>
+      </c>
+      <c r="B368" s="2">
+        <v>0.50347222222222221</v>
+      </c>
+      <c r="D368">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="369" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A369" s="1">
+        <v>44617</v>
+      </c>
+      <c r="B369" s="2">
+        <v>0.53194444444444444</v>
+      </c>
+      <c r="D369">
+        <v>1</v>
+      </c>
+      <c r="F369">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="370" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A370" s="1">
+        <v>44617</v>
+      </c>
+      <c r="B370" s="2">
+        <v>0.67708333333333337</v>
+      </c>
+      <c r="C370">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="371" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A371" s="1">
+        <v>44617</v>
+      </c>
+      <c r="B371" s="2">
+        <v>0.7909722222222223</v>
+      </c>
+      <c r="C371">
+        <v>1</v>
+      </c>
+      <c r="F371">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="372" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A372" s="1">
+        <v>44617</v>
+      </c>
+      <c r="B372" s="2">
+        <v>0.79513888888888884</v>
+      </c>
+      <c r="D372">
+        <v>1</v>
+      </c>
+      <c r="F372">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="373" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A373" s="1">
+        <v>44617</v>
+      </c>
+      <c r="B373" s="2">
+        <v>0.80694444444444446</v>
+      </c>
+      <c r="E373">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="374" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A374" s="1">
+        <v>44618</v>
+      </c>
+      <c r="B374" s="2">
+        <v>0.38194444444444442</v>
+      </c>
+      <c r="C374">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="375" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A375" s="1">
+        <v>44618</v>
+      </c>
+      <c r="B375" s="2">
+        <v>0.39861111111111108</v>
+      </c>
+      <c r="E375">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="376" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A376" s="1">
+        <v>44618</v>
+      </c>
+      <c r="B376" s="2">
+        <v>0.46180555555555558</v>
+      </c>
+      <c r="D376">
+        <v>1</v>
+      </c>
+      <c r="F376">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="377" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A377" s="1">
+        <v>44618</v>
+      </c>
+      <c r="B377" s="2">
+        <v>0.47430555555555554</v>
+      </c>
+      <c r="D377">
+        <v>1</v>
+      </c>
+      <c r="F377">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="378" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A378" s="1">
+        <v>44618</v>
+      </c>
+      <c r="B378" s="2">
+        <v>0.62847222222222221</v>
+      </c>
+      <c r="C378">
+        <v>1</v>
+      </c>
+      <c r="F378">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="379" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A379" s="1">
+        <v>44618</v>
+      </c>
+      <c r="B379" s="2">
+        <v>0.78472222222222221</v>
+      </c>
+      <c r="C379">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="380" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A380" s="1">
+        <v>44618</v>
+      </c>
+      <c r="B380" s="2">
+        <v>0.79166666666666663</v>
+      </c>
+      <c r="E380">
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
update out the number / rate of toilet out
</commit_message>
<xml_diff>
--- a/baron_log.xlsx
+++ b/baron_log.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24931"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\seito\Documents\Baron-log\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{01517528-37B5-4FB0-A772-D6CB610A0C9E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{67DC5DD6-CC1F-4B8A-B8C9-9D8E3283D7A9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
   <si>
     <t>date</t>
   </si>
@@ -44,14 +44,6 @@
   </si>
   <si>
     <t>Gohan</t>
-  </si>
-  <si>
-    <t>i</t>
-    <phoneticPr fontId="18"/>
-  </si>
-  <si>
-    <t>o</t>
-    <phoneticPr fontId="18"/>
   </si>
   <si>
     <t>notes</t>
@@ -1028,11 +1020,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G380"/>
+  <dimension ref="A1:G470"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A365" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18" x14ac:dyDescent="0.55000000000000004"/>
@@ -1059,10 +1051,10 @@
         <v>4</v>
       </c>
       <c r="F1" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="G1" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.55000000000000004">
@@ -2981,7 +2973,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="177" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="177" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A177" s="1">
         <v>44527</v>
       </c>
@@ -2992,7 +2984,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="178" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="178" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A178" s="1">
         <v>44527</v>
       </c>
@@ -3003,7 +2995,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="179" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="179" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A179" s="1">
         <v>44527</v>
       </c>
@@ -3014,7 +3006,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="180" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="180" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A180" s="1">
         <v>44527</v>
       </c>
@@ -3025,7 +3017,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="181" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="181" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A181" s="1">
         <v>44528</v>
       </c>
@@ -3036,7 +3028,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="182" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="182" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A182" s="1">
         <v>44528</v>
       </c>
@@ -3047,7 +3039,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="183" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="183" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A183" s="1">
         <v>44528</v>
       </c>
@@ -3058,7 +3050,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="184" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="184" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A184" s="1">
         <v>44528</v>
       </c>
@@ -3069,7 +3061,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="185" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="185" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A185" s="1">
         <v>44528</v>
       </c>
@@ -3080,7 +3072,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="186" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="186" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A186" s="1">
         <v>44528</v>
       </c>
@@ -3090,11 +3082,8 @@
       <c r="C186">
         <v>1</v>
       </c>
-      <c r="F186" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="187" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    </row>
+    <row r="187" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A187" s="1">
         <v>44528</v>
       </c>
@@ -3105,7 +3094,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="188" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="188" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A188" s="1">
         <v>44528</v>
       </c>
@@ -3116,7 +3105,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="189" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="189" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A189" s="1">
         <v>44528</v>
       </c>
@@ -3127,7 +3116,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="190" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="190" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A190" s="1">
         <v>44528</v>
       </c>
@@ -3138,7 +3127,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="191" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="191" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A191" s="1">
         <v>44528</v>
       </c>
@@ -3149,7 +3138,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="192" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="192" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A192" s="1">
         <v>44529</v>
       </c>
@@ -3500,8 +3489,8 @@
       <c r="D223">
         <v>1</v>
       </c>
-      <c r="F223" t="s">
-        <v>6</v>
+      <c r="F223">
+        <v>1</v>
       </c>
     </row>
     <row r="224" spans="1:6" x14ac:dyDescent="0.55000000000000004">
@@ -3514,8 +3503,8 @@
       <c r="C224">
         <v>1</v>
       </c>
-      <c r="F224" t="s">
-        <v>6</v>
+      <c r="F224">
+        <v>1</v>
       </c>
     </row>
     <row r="225" spans="1:7" x14ac:dyDescent="0.55000000000000004">
@@ -3594,8 +3583,8 @@
       <c r="D231">
         <v>1</v>
       </c>
-      <c r="F231" t="s">
-        <v>6</v>
+      <c r="F231">
+        <v>1</v>
       </c>
     </row>
     <row r="232" spans="1:7" x14ac:dyDescent="0.55000000000000004">
@@ -3620,7 +3609,7 @@
         <v>0</v>
       </c>
       <c r="G233" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
     <row r="234" spans="1:7" x14ac:dyDescent="0.55000000000000004">
@@ -3656,7 +3645,7 @@
         <v>0</v>
       </c>
       <c r="G236" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
     </row>
     <row r="237" spans="1:7" x14ac:dyDescent="0.55000000000000004">
@@ -3724,8 +3713,8 @@
       <c r="C242">
         <v>1</v>
       </c>
-      <c r="F242" t="s">
-        <v>6</v>
+      <c r="F242">
+        <v>1</v>
       </c>
     </row>
     <row r="243" spans="1:6" x14ac:dyDescent="0.55000000000000004">
@@ -3738,8 +3727,8 @@
       <c r="D243">
         <v>1</v>
       </c>
-      <c r="F243" t="s">
-        <v>6</v>
+      <c r="F243">
+        <v>1</v>
       </c>
     </row>
     <row r="244" spans="1:6" x14ac:dyDescent="0.55000000000000004">
@@ -3818,8 +3807,8 @@
       <c r="D250">
         <v>1</v>
       </c>
-      <c r="F250" t="s">
-        <v>6</v>
+      <c r="F250">
+        <v>1</v>
       </c>
     </row>
     <row r="251" spans="1:6" x14ac:dyDescent="0.55000000000000004">
@@ -3887,8 +3876,8 @@
       <c r="C256">
         <v>1</v>
       </c>
-      <c r="F256" t="s">
-        <v>6</v>
+      <c r="F256">
+        <v>1</v>
       </c>
     </row>
     <row r="257" spans="1:6" x14ac:dyDescent="0.55000000000000004">
@@ -5306,6 +5295,1071 @@
         <v>0.79166666666666663</v>
       </c>
       <c r="E380">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="381" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A381" s="1">
+        <v>44618</v>
+      </c>
+      <c r="B381" s="2">
+        <v>0.38194444444444442</v>
+      </c>
+      <c r="C381">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="382" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A382" s="1">
+        <v>44618</v>
+      </c>
+      <c r="B382" s="2">
+        <v>0.39861111111111108</v>
+      </c>
+      <c r="E382">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="383" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A383" s="1">
+        <v>44618</v>
+      </c>
+      <c r="B383" s="2">
+        <v>0.46180555555555558</v>
+      </c>
+      <c r="D383">
+        <v>1</v>
+      </c>
+      <c r="F383">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="384" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A384" s="1">
+        <v>44618</v>
+      </c>
+      <c r="B384" s="2">
+        <v>0.47430555555555554</v>
+      </c>
+      <c r="D384">
+        <v>1</v>
+      </c>
+      <c r="F384">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="385" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A385" s="1">
+        <v>44618</v>
+      </c>
+      <c r="B385" s="2">
+        <v>0.62847222222222221</v>
+      </c>
+      <c r="C385">
+        <v>1</v>
+      </c>
+      <c r="F385">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="386" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A386" s="1">
+        <v>44618</v>
+      </c>
+      <c r="B386" s="2">
+        <v>0.77083333333333337</v>
+      </c>
+      <c r="C386">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="387" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A387" s="1">
+        <v>44618</v>
+      </c>
+      <c r="B387" s="2">
+        <v>0.79166666666666663</v>
+      </c>
+      <c r="E387">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="388" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A388" s="1">
+        <v>44619</v>
+      </c>
+      <c r="B388" s="2">
+        <v>0.38194444444444442</v>
+      </c>
+      <c r="C388">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="389" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A389" s="1">
+        <v>44619</v>
+      </c>
+      <c r="B389" s="2">
+        <v>0.40277777777777773</v>
+      </c>
+      <c r="C389">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="390" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A390" s="1">
+        <v>44619</v>
+      </c>
+      <c r="B390" s="2">
+        <v>0.42569444444444443</v>
+      </c>
+      <c r="D390">
+        <v>1</v>
+      </c>
+      <c r="F390">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="391" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A391" s="1">
+        <v>44619</v>
+      </c>
+      <c r="B391" s="2">
+        <v>0.45416666666666666</v>
+      </c>
+      <c r="C391">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="392" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A392" s="1">
+        <v>44619</v>
+      </c>
+      <c r="B392" s="2">
+        <v>0.47500000000000003</v>
+      </c>
+      <c r="E392">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="393" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A393" s="1">
+        <v>44619</v>
+      </c>
+      <c r="B393" s="2">
+        <v>0.87847222222222221</v>
+      </c>
+      <c r="C393">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="394" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A394" s="1">
+        <v>44619</v>
+      </c>
+      <c r="B394" s="2">
+        <v>0.93402777777777779</v>
+      </c>
+      <c r="C394">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="395" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A395" s="1">
+        <v>44619</v>
+      </c>
+      <c r="B395" s="2">
+        <v>0.95486111111111116</v>
+      </c>
+      <c r="D395">
+        <v>1</v>
+      </c>
+      <c r="F395">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="396" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A396" s="1">
+        <v>44620</v>
+      </c>
+      <c r="B396" s="2">
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="C396">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="397" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A397" s="1">
+        <v>44620</v>
+      </c>
+      <c r="B397" s="2">
+        <v>0.35416666666666669</v>
+      </c>
+      <c r="E397">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="398" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A398" s="1">
+        <v>44620</v>
+      </c>
+      <c r="B398" s="2">
+        <v>0.60069444444444442</v>
+      </c>
+      <c r="C398">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="399" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A399" s="1">
+        <v>44620</v>
+      </c>
+      <c r="B399" s="2">
+        <v>0.81944444444444453</v>
+      </c>
+      <c r="E399">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="400" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A400" s="1">
+        <v>44620</v>
+      </c>
+      <c r="B400" s="2">
+        <v>0.88888888888888884</v>
+      </c>
+      <c r="C400">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="401" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A401" s="1">
+        <v>44620</v>
+      </c>
+      <c r="B401" s="2">
+        <v>0.91319444444444453</v>
+      </c>
+      <c r="C401">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="402" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A402" s="1">
+        <v>44620</v>
+      </c>
+      <c r="B402" s="2">
+        <v>0.92361111111111116</v>
+      </c>
+      <c r="D402">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="403" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A403" s="1">
+        <v>44621</v>
+      </c>
+      <c r="B403" s="2">
+        <v>0.35416666666666669</v>
+      </c>
+      <c r="C403">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="404" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A404" s="1">
+        <v>44621</v>
+      </c>
+      <c r="B404" s="2">
+        <v>0.39930555555555558</v>
+      </c>
+      <c r="C404">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="405" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A405" s="1">
+        <v>44621</v>
+      </c>
+      <c r="B405" s="2">
+        <v>0.40208333333333335</v>
+      </c>
+      <c r="D405">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="406" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A406" s="1">
+        <v>44621</v>
+      </c>
+      <c r="B406" s="2">
+        <v>0.4055555555555555</v>
+      </c>
+      <c r="E406">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="407" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A407" s="1">
+        <v>44621</v>
+      </c>
+      <c r="B407" s="2">
+        <v>0.71527777777777779</v>
+      </c>
+      <c r="C407">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="408" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A408" s="1">
+        <v>44621</v>
+      </c>
+      <c r="B408" s="2">
+        <v>0.80902777777777779</v>
+      </c>
+      <c r="C408">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="409" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A409" s="1">
+        <v>44621</v>
+      </c>
+      <c r="B409" s="2">
+        <v>0.91875000000000007</v>
+      </c>
+      <c r="D409">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="410" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A410" s="1">
+        <v>44622</v>
+      </c>
+      <c r="B410" s="2">
+        <v>0.3611111111111111</v>
+      </c>
+      <c r="C410">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="411" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A411" s="1">
+        <v>44622</v>
+      </c>
+      <c r="B411" s="2">
+        <v>0.37083333333333335</v>
+      </c>
+      <c r="E411">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="412" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A412" s="1">
+        <v>44622</v>
+      </c>
+      <c r="B412" s="2">
+        <v>0.4826388888888889</v>
+      </c>
+      <c r="C412">
+        <v>1</v>
+      </c>
+      <c r="F412">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="413" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A413" s="1">
+        <v>44622</v>
+      </c>
+      <c r="B413" s="2">
+        <v>0.48749999999999999</v>
+      </c>
+      <c r="D413">
+        <v>1</v>
+      </c>
+      <c r="F413">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="414" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A414" s="1">
+        <v>44622</v>
+      </c>
+      <c r="B414" s="2">
+        <v>0.63541666666666663</v>
+      </c>
+      <c r="C414">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="415" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A415" s="1">
+        <v>44622</v>
+      </c>
+      <c r="B415" s="2">
+        <v>0.77083333333333337</v>
+      </c>
+      <c r="E415">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="416" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A416" s="1">
+        <v>44622</v>
+      </c>
+      <c r="B416" s="2">
+        <v>0.91875000000000007</v>
+      </c>
+      <c r="C416">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="417" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A417" s="1">
+        <v>44622</v>
+      </c>
+      <c r="B417" s="2">
+        <v>0.9277777777777777</v>
+      </c>
+      <c r="D417">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="418" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A418" s="1">
+        <v>44622</v>
+      </c>
+      <c r="B418" s="2">
+        <v>0.35138888888888892</v>
+      </c>
+      <c r="C418">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="419" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A419" s="1">
+        <v>44622</v>
+      </c>
+      <c r="B419" s="2">
+        <v>0.35486111111111113</v>
+      </c>
+      <c r="E419">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="420" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A420" s="1">
+        <v>44622</v>
+      </c>
+      <c r="B420" s="2">
+        <v>0.4236111111111111</v>
+      </c>
+      <c r="C420">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="421" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A421" s="1">
+        <v>44622</v>
+      </c>
+      <c r="B421" s="2">
+        <v>0.42777777777777781</v>
+      </c>
+      <c r="D421">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="422" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A422" s="1">
+        <v>44622</v>
+      </c>
+      <c r="B422" s="2">
+        <v>0.55208333333333337</v>
+      </c>
+      <c r="C422">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="423" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A423" s="1">
+        <v>44622</v>
+      </c>
+      <c r="B423" s="2">
+        <v>0.76736111111111116</v>
+      </c>
+      <c r="C423">
+        <v>1</v>
+      </c>
+      <c r="F423">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="424" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A424" s="1">
+        <v>44623</v>
+      </c>
+      <c r="B424" s="2">
+        <v>0.34027777777777773</v>
+      </c>
+      <c r="C424">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="425" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A425" s="1">
+        <v>44623</v>
+      </c>
+      <c r="B425" s="2">
+        <v>0.37916666666666665</v>
+      </c>
+      <c r="D425">
+        <v>1</v>
+      </c>
+      <c r="F425">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="426" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A426" s="1">
+        <v>44623</v>
+      </c>
+      <c r="B426" s="2">
+        <v>0.3888888888888889</v>
+      </c>
+      <c r="E426">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="427" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A427" s="1">
+        <v>44623</v>
+      </c>
+      <c r="B427" s="2">
+        <v>0.70833333333333337</v>
+      </c>
+      <c r="C427">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="428" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A428" s="1">
+        <v>44623</v>
+      </c>
+      <c r="B428" s="2">
+        <v>0.79236111111111107</v>
+      </c>
+      <c r="C428">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="429" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A429" s="1">
+        <v>44623</v>
+      </c>
+      <c r="B429" s="2">
+        <v>0.80555555555555547</v>
+      </c>
+      <c r="E429">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="430" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A430" s="1">
+        <v>44623</v>
+      </c>
+      <c r="B430" s="2">
+        <v>0.90555555555555556</v>
+      </c>
+      <c r="C430">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="431" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A431" s="1">
+        <v>44623</v>
+      </c>
+      <c r="B431" s="2">
+        <v>0.91180555555555554</v>
+      </c>
+      <c r="D431">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="432" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A432" s="1">
+        <v>44624</v>
+      </c>
+      <c r="B432" s="2">
+        <v>0.39583333333333331</v>
+      </c>
+      <c r="C432">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="433" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A433" s="1">
+        <v>44624</v>
+      </c>
+      <c r="B433" s="2">
+        <v>0.40625</v>
+      </c>
+      <c r="E433">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="434" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A434" s="1">
+        <v>44624</v>
+      </c>
+      <c r="B434" s="2">
+        <v>0.47291666666666665</v>
+      </c>
+      <c r="C434">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="435" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A435" s="1">
+        <v>44624</v>
+      </c>
+      <c r="B435" s="2">
+        <v>0.47638888888888892</v>
+      </c>
+      <c r="D435">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="436" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A436" s="1">
+        <v>44624</v>
+      </c>
+      <c r="B436" s="2">
+        <v>0.59583333333333333</v>
+      </c>
+      <c r="C436">
+        <v>1</v>
+      </c>
+      <c r="F436">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="437" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A437" s="1">
+        <v>44624</v>
+      </c>
+      <c r="B437" s="2">
+        <v>0.60069444444444442</v>
+      </c>
+      <c r="D437">
+        <v>1</v>
+      </c>
+      <c r="F437">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="438" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A438" s="1">
+        <v>44624</v>
+      </c>
+      <c r="B438" s="2">
+        <v>0.68194444444444446</v>
+      </c>
+      <c r="C438">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="439" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A439" s="1">
+        <v>44624</v>
+      </c>
+      <c r="B439" s="2">
+        <v>0.80486111111111114</v>
+      </c>
+      <c r="E439">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="440" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A440" s="1">
+        <v>44624</v>
+      </c>
+      <c r="B440" s="2">
+        <v>0.90486111111111101</v>
+      </c>
+      <c r="C440">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="441" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A441" s="1">
+        <v>44625</v>
+      </c>
+      <c r="B441" s="2">
+        <v>0.39583333333333331</v>
+      </c>
+      <c r="C441">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="442" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A442" s="1">
+        <v>44625</v>
+      </c>
+      <c r="B442" s="2">
+        <v>0.40625</v>
+      </c>
+      <c r="E442">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="443" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A443" s="1">
+        <v>44625</v>
+      </c>
+      <c r="B443" s="2">
+        <v>0.47291666666666665</v>
+      </c>
+      <c r="C443">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="444" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A444" s="1">
+        <v>44625</v>
+      </c>
+      <c r="B444" s="2">
+        <v>0.47638888888888892</v>
+      </c>
+      <c r="D444">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="445" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A445" s="1">
+        <v>44625</v>
+      </c>
+      <c r="B445" s="2">
+        <v>0.59583333333333333</v>
+      </c>
+      <c r="C445">
+        <v>1</v>
+      </c>
+      <c r="F445">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="446" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A446" s="1">
+        <v>44625</v>
+      </c>
+      <c r="B446" s="2">
+        <v>0.60069444444444442</v>
+      </c>
+      <c r="D446">
+        <v>1</v>
+      </c>
+      <c r="F446">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="447" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A447" s="1">
+        <v>44625</v>
+      </c>
+      <c r="B447" s="2">
+        <v>0.68194444444444446</v>
+      </c>
+      <c r="C447">
+        <v>1</v>
+      </c>
+      <c r="F447">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="448" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A448" s="1">
+        <v>44625</v>
+      </c>
+      <c r="B448" s="2">
+        <v>0.80486111111111114</v>
+      </c>
+      <c r="E448">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="449" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A449" s="1">
+        <v>44625</v>
+      </c>
+      <c r="B449" s="2">
+        <v>0.90486111111111101</v>
+      </c>
+      <c r="C449">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="450" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A450" s="1">
+        <v>44626</v>
+      </c>
+      <c r="B450" s="2">
+        <v>0.3923611111111111</v>
+      </c>
+      <c r="C450">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="451" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A451" s="1">
+        <v>44626</v>
+      </c>
+      <c r="B451" s="2">
+        <v>0.40625</v>
+      </c>
+      <c r="E451">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="452" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A452" s="1">
+        <v>44626</v>
+      </c>
+      <c r="B452" s="2">
+        <v>0.51944444444444449</v>
+      </c>
+      <c r="C452">
+        <v>1</v>
+      </c>
+      <c r="F452">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="453" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A453" s="1">
+        <v>44626</v>
+      </c>
+      <c r="B453" s="2">
+        <v>0.52222222222222225</v>
+      </c>
+      <c r="D453">
+        <v>1</v>
+      </c>
+      <c r="F453">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="454" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A454" s="1">
+        <v>44626</v>
+      </c>
+      <c r="B454" s="2">
+        <v>0.52638888888888891</v>
+      </c>
+      <c r="D454">
+        <v>1</v>
+      </c>
+      <c r="F454">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="455" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A455" s="1">
+        <v>44626</v>
+      </c>
+      <c r="B455" s="2">
+        <v>0.52986111111111112</v>
+      </c>
+      <c r="D455">
+        <v>1</v>
+      </c>
+      <c r="F455">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="456" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A456" s="1">
+        <v>44626</v>
+      </c>
+      <c r="B456" s="2">
+        <v>0.5805555555555556</v>
+      </c>
+      <c r="C456">
+        <v>1</v>
+      </c>
+      <c r="F456">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="457" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A457" s="1">
+        <v>44626</v>
+      </c>
+      <c r="B457" s="2">
+        <v>0.58194444444444449</v>
+      </c>
+      <c r="C457">
+        <v>1</v>
+      </c>
+      <c r="F457">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="458" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A458" s="1">
+        <v>44626</v>
+      </c>
+      <c r="B458" s="2">
+        <v>0.74305555555555547</v>
+      </c>
+      <c r="C458">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="459" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A459" s="1">
+        <v>44626</v>
+      </c>
+      <c r="B459" s="2">
+        <v>0.79513888888888884</v>
+      </c>
+      <c r="C459">
+        <v>1</v>
+      </c>
+      <c r="F459">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="460" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A460" s="1">
+        <v>44626</v>
+      </c>
+      <c r="B460" s="2">
+        <v>0.80902777777777779</v>
+      </c>
+      <c r="E460">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="461" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A461" s="1">
+        <v>44626</v>
+      </c>
+      <c r="B461" s="2">
+        <v>0.91875000000000007</v>
+      </c>
+      <c r="C461">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="462" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A462" s="1">
+        <v>44627</v>
+      </c>
+      <c r="B462" s="2">
+        <v>0.31944444444444448</v>
+      </c>
+      <c r="C462">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="463" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A463" s="1">
+        <v>44627</v>
+      </c>
+      <c r="B463" s="2">
+        <v>0.33611111111111108</v>
+      </c>
+      <c r="C463">
+        <v>1</v>
+      </c>
+      <c r="F463">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="464" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A464" s="1">
+        <v>44627</v>
+      </c>
+      <c r="B464" s="2">
+        <v>0.3611111111111111</v>
+      </c>
+      <c r="E464">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="465" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A465" s="1">
+        <v>44627</v>
+      </c>
+      <c r="B465" s="2">
+        <v>0.45416666666666666</v>
+      </c>
+      <c r="C465">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="466" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A466" s="1">
+        <v>44627</v>
+      </c>
+      <c r="B466" s="2">
+        <v>0.60625000000000007</v>
+      </c>
+      <c r="C466">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="467" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A467" s="1">
+        <v>44627</v>
+      </c>
+      <c r="B467" s="2">
+        <v>0.75347222222222221</v>
+      </c>
+      <c r="C467">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="468" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A468" s="1">
+        <v>44627</v>
+      </c>
+      <c r="B468" s="2">
+        <v>0.77083333333333337</v>
+      </c>
+      <c r="C468">
+        <v>1</v>
+      </c>
+      <c r="F468">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="469" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A469" s="1">
+        <v>44627</v>
+      </c>
+      <c r="B469" s="2">
+        <v>0.77777777777777779</v>
+      </c>
+      <c r="D469">
+        <v>1</v>
+      </c>
+      <c r="F469">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="470" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A470" s="1">
+        <v>44627</v>
+      </c>
+      <c r="B470" s="2">
+        <v>0.78472222222222221</v>
+      </c>
+      <c r="D470">
+        <v>1</v>
+      </c>
+      <c r="F470">
         <v>1</v>
       </c>
     </row>

</xml_diff>